<commit_message>
[AGR] Add stats: 23
</commit_message>
<xml_diff>
--- a/Agranari/AgranariAdventures_Characters.xlsx
+++ b/Agranari/AgranariAdventures_Characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Stories\DnD-Stories\Agranari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F652582D-25AE-4551-9744-F9EA53FEF50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8C77B4-A5F1-4D59-9E4B-C03447782D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{B9DB5469-233B-4BC4-B3BA-52FF33A82184}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="69">
   <si>
     <t>Tools</t>
   </si>
@@ -204,6 +204,48 @@
   </si>
   <si>
     <t>SoftMaxBendingRange</t>
+  </si>
+  <si>
+    <t>SignatureSpellDifficultyReduction</t>
+  </si>
+  <si>
+    <t>1d100 (Disadv)</t>
+  </si>
+  <si>
+    <t>SpellDifficulty</t>
+  </si>
+  <si>
+    <t>IsSignatureSpell?</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>SpellDifficultyCastTimeIncrease</t>
+  </si>
+  <si>
+    <t>SpellDifficultyCastRangeReduction</t>
+  </si>
+  <si>
+    <t>Buff Ability Score</t>
+  </si>
+  <si>
+    <t>Spell Fluency Variables</t>
+  </si>
+  <si>
+    <t>MaxStableHoofChain</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>BendLargeTargetRange</t>
+  </si>
+  <si>
+    <t>SelfBonusBendingPower</t>
+  </si>
+  <si>
+    <t>TargetingSelf?</t>
   </si>
 </sst>
 </file>
@@ -211,7 +253,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -282,25 +324,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,11 +680,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -845,11 +886,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1047,11 +1088,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1229,16 +1270,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134592FA-46C7-4490-B8BE-DC20D051C225}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.19921875" bestFit="1" customWidth="1"/>
@@ -1247,10 +1288,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="5"/>
       <c r="C1" t="s">
         <v>30</v>
       </c>
@@ -1259,22 +1300,22 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1287,14 +1328,14 @@
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="13"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
@@ -1319,14 +1360,20 @@
         <v>45</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3">
         <f>(C5+20)/240</f>
-        <v>8.7499999999999994E-2</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1337,11 +1384,11 @@
         <v>44</v>
       </c>
       <c r="C6" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <f>C6+D4</f>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
         <v>38</v>
@@ -1350,122 +1397,194 @@
         <v>53</v>
       </c>
       <c r="J6">
-        <f>(IF(H7=0,D11,1))</f>
-        <v>1.8</v>
+        <f>(IF(H8=0,D12,1))+IF(H5="y",D13,0)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="8">
-        <v>7</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C7" s="2"/>
       <c r="D7">
-        <f>C7*5</f>
-        <v>35</v>
+        <f>C7</f>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="9">
-        <f>(D4-(H7/D7))*J6</f>
-        <v>10.8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <f>C8*5</f>
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="D8">
-        <f>MAX(1,23-(D4+C8))</f>
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="7">
+        <f>(D4-(H8/D8))*J6</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <f>MAX(1,23-(D4+C9))</f>
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="G8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="10">
-        <f>IF(J7&gt;0,ROUNDDOWN((D4/J7)*D8,0),"OoB")</f>
-        <v>4</v>
-      </c>
-      <c r="K8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8">
-        <f>IF(J7&gt;0,J8*6/60,"OoB")</f>
-        <v>0.4</v>
-      </c>
-      <c r="M8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9">
-        <f>(D4-1)*D7</f>
-        <v>175</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
       <c r="G9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="12">
-        <f>IF(J7&gt;0,1/J8,0)</f>
-        <v>0.25</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="11"/>
+        <v>54</v>
+      </c>
       <c r="D10">
-        <f>D4*D7</f>
-        <v>210</v>
+        <f>(D4-1)*D8</f>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11">
+        <f>D4*D8</f>
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="8">
+        <f>IF(J8&gt;0,ROUNDDOWN((D4/J8)*D9,0),"OoB")</f>
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11">
+        <f>IF(J8&gt;0,J11*6/60,"OoB")</f>
+        <v>0.1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="2">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <f>(C11/5)+1</f>
-        <v>1.8</v>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f>(C12/5)+1</f>
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="9">
+        <f>IF(J8&gt;0,1/J11,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14">
+        <f>C14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[AGR] Character stats update*
*including:
- 23 (I think)
- Tracker Shurlekt
</commit_message>
<xml_diff>
--- a/Agranari/AgranariAdventures_Characters.xlsx
+++ b/Agranari/AgranariAdventures_Characters.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Stories\DnD-Stories\Agranari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8C77B4-A5F1-4D59-9E4B-C03447782D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FCEDE1-82E6-42D9-AD3F-238994B63519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{B9DB5469-233B-4BC4-B3BA-52FF33A82184}"/>
   </bookViews>
   <sheets>
-    <sheet name="Zaja" sheetId="1" r:id="rId1"/>
+    <sheet name="Zajar" sheetId="1" r:id="rId1"/>
     <sheet name="Grarthta" sheetId="2" r:id="rId2"/>
     <sheet name="Rafrol" sheetId="3" r:id="rId3"/>
     <sheet name="23" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="70">
   <si>
     <t>Tools</t>
   </si>
@@ -110,9 +111,6 @@
     <t>Bear</t>
   </si>
   <si>
-    <t>Zaja Zernam</t>
-  </si>
-  <si>
     <t>Grarthta</t>
   </si>
   <si>
@@ -140,9 +138,6 @@
     <t>BendingPower</t>
   </si>
   <si>
-    <t>HoofLength</t>
-  </si>
-  <si>
     <t>HoofLife</t>
   </si>
   <si>
@@ -164,12 +159,6 @@
     <t>DistancePerBendingPowerReduction</t>
   </si>
   <si>
-    <t>DistantBendCastTime</t>
-  </si>
-  <si>
-    <t>DistantBendPower</t>
-  </si>
-  <si>
     <t>Die</t>
   </si>
   <si>
@@ -188,9 +177,6 @@
     <t>MaxBendingRange</t>
   </si>
   <si>
-    <t>DistantBendPercentAdd</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
@@ -200,24 +186,12 @@
     <t>1d10 (Disadv)</t>
   </si>
   <si>
-    <t>BonusBendPower</t>
-  </si>
-  <si>
     <t>SoftMaxBendingRange</t>
   </si>
   <si>
-    <t>SignatureSpellDifficultyReduction</t>
-  </si>
-  <si>
-    <t>1d100 (Disadv)</t>
-  </si>
-  <si>
     <t>SpellDifficulty</t>
   </si>
   <si>
-    <t>IsSignatureSpell?</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -233,12 +207,6 @@
     <t>Spell Fluency Variables</t>
   </si>
   <si>
-    <t>MaxStableHoofChain</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
     <t>BendLargeTargetRange</t>
   </si>
   <si>
@@ -246,6 +214,42 @@
   </si>
   <si>
     <t>TargetingSelf?</t>
+  </si>
+  <si>
+    <t>CastDistance</t>
+  </si>
+  <si>
+    <t>SpellFluency</t>
+  </si>
+  <si>
+    <t>Zajar Zernam</t>
+  </si>
+  <si>
+    <t>Final Hoof Length</t>
+  </si>
+  <si>
+    <t>Percent Add Per Round</t>
+  </si>
+  <si>
+    <t>Cast Time</t>
+  </si>
+  <si>
+    <t>Bonus BendPower</t>
+  </si>
+  <si>
+    <t>Total BendPower</t>
+  </si>
+  <si>
+    <t>Base Cast Time</t>
+  </si>
+  <si>
+    <t>HoofGrowthPerRound</t>
+  </si>
+  <si>
+    <t>MaxStableHoofLength</t>
+  </si>
+  <si>
+    <t>1d100 (Ax1, Dx2)</t>
   </si>
 </sst>
 </file>
@@ -255,7 +259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +278,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -324,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -332,8 +343,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -341,6 +350,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -660,7 +672,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:H3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -670,21 +682,21 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -760,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2">
         <v>13</v>
@@ -876,21 +888,21 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -988,7 +1000,7 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -1032,7 +1044,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1078,21 +1090,21 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1168,7 +1180,7 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2">
         <v>11</v>
@@ -1270,16 +1282,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134592FA-46C7-4490-B8BE-DC20D051C225}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.19921875" bestFit="1" customWidth="1"/>
@@ -1289,31 +1301,31 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -1328,21 +1340,21 @@
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="11"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2">
         <v>6</v>
@@ -1354,75 +1366,89 @@
     </row>
     <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2">
         <v>22</v>
       </c>
       <c r="D5" s="3">
-        <f>(C5+20)/240</f>
-        <v>0.17499999999999999</v>
+        <f>(100-C5+20)/240</f>
+        <v>0.40833333333333333</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C6" s="2">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="D6">
-        <f>C6+D4</f>
+        <f>5*C6/100</f>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6">
-        <f>(IF(H8=0,D12,1))+IF(H5="y",D13,0)</f>
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
       <c r="D7">
-        <f>C7</f>
-        <v>0</v>
+        <f>C7+D4</f>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="2">
+        <v>100</v>
+      </c>
+      <c r="J7" s="10">
+        <f>H7-H8</f>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
@@ -1435,25 +1461,22 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="7">
-        <f>(D4-(H8/D8))*J6</f>
-        <v>42</v>
+      <c r="J8" s="10">
+        <f>(1+(J7/100))</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>
@@ -1463,16 +1486,24 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>37</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10">
+        <f>(IF(H6=0,D12,1))+IF(H5="y",D13,0)</f>
+        <v>7</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D10">
         <f>(D4-1)*D8</f>
@@ -1481,16 +1512,22 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="G10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11">
+        <f>(D4-(J8*H6/D8))*J9</f>
+        <v>42</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <f>D4*D8</f>
@@ -1499,30 +1536,32 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="8">
-        <f>IF(J8&gt;0,ROUNDDOWN((D4/J8)*D9,0),"OoB")</f>
+      <c r="G11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="12">
+        <f>IF(J10&gt;0,ROUNDDOWN((D4/J10)*D9,0),"OoB")</f>
         <v>1</v>
       </c>
-      <c r="K11" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11">
-        <f>IF(J8&gt;0,J11*6/60,"OoB")</f>
+      <c r="K11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="10">
+        <f>IF(J10&gt;0,J11*6/60,"OoB")</f>
         <v>0.1</v>
       </c>
-      <c r="M11" t="s">
-        <v>50</v>
+      <c r="M11" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -1532,59 +1571,71 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="9">
-        <f>IF(J8&gt;0,1/J11,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>63</v>
+      </c>
+      <c r="J12">
+        <f>IF(J10&gt;0,ROUNDDOWN(MAX(1,J11*J8),0),"OoB")</f>
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12">
+        <f>IF(J10&gt;0,J12*6/60,"OoB")</f>
+        <v>0.2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="12"/>
+        <v>56</v>
+      </c>
       <c r="D13">
         <v>5</v>
       </c>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="7">
+        <f>IF(J10&gt;0,1/J11,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14">
-        <f>C14</f>
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14">
+        <f>J12*D5</f>
+        <v>0.81666666666666665</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C17" s="13"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[AGR] Add character: Fenrir
</commit_message>
<xml_diff>
--- a/Agranari/AgranariAdventures_Characters.xlsx
+++ b/Agranari/AgranariAdventures_Characters.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Stories\DnD-Stories\Agranari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C53AED5-4AAC-410C-AC27-9A05AAC0FB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E160F0-CE7D-4293-A5E1-CA40EE5B891C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{B9DB5469-233B-4BC4-B3BA-52FF33A82184}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{B9DB5469-233B-4BC4-B3BA-52FF33A82184}"/>
   </bookViews>
   <sheets>
     <sheet name="Zajar" sheetId="1" r:id="rId1"/>
     <sheet name="Grarthta" sheetId="2" r:id="rId2"/>
     <sheet name="Rafrol" sheetId="3" r:id="rId3"/>
-    <sheet name="23" sheetId="4" r:id="rId4"/>
-    <sheet name="Tracker Shurlekt" sheetId="5" r:id="rId5"/>
-    <sheet name="Wolf Goon" sheetId="6" r:id="rId6"/>
+    <sheet name="Zemorsin" sheetId="4" r:id="rId4"/>
+    <sheet name="Fenrir" sheetId="7" r:id="rId5"/>
+    <sheet name="Tracker Shurlekt" sheetId="5" r:id="rId6"/>
+    <sheet name="Wolf Goon" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="157">
   <si>
     <t>Tools</t>
   </si>
@@ -146,9 +146,6 @@
     <t>BendCastTime</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
@@ -405,14 +402,126 @@
   </si>
   <si>
     <t>LickWoundsHeal</t>
+  </si>
+  <si>
+    <t>Silent Step</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>-7, -6, -5, -4, -3, -2, -1, 0</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>hide from doe on road</t>
+  </si>
+  <si>
+    <t>hide in bushes near ranch</t>
+  </si>
+  <si>
+    <t>hide in weeds next to silo</t>
+  </si>
+  <si>
+    <t>Change Size</t>
+  </si>
+  <si>
+    <t>shrink to 30% size to go under porch</t>
+  </si>
+  <si>
+    <t>hide in bush from gra</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Total Difficulty</t>
+  </si>
+  <si>
+    <t>Percent Complete</t>
+  </si>
+  <si>
+    <t>Hoof Length</t>
+  </si>
+  <si>
+    <t>Zemorsin</t>
+  </si>
+  <si>
+    <t>in.</t>
+  </si>
+  <si>
+    <t>Minor Camouflage</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Fluency</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Active Spells</t>
+  </si>
+  <si>
+    <t>FIrePower</t>
+  </si>
+  <si>
+    <t>FireCost</t>
+  </si>
+  <si>
+    <t>FirePoints</t>
+  </si>
+  <si>
+    <t>FireDamage</t>
+  </si>
+  <si>
+    <t>WillPower</t>
+  </si>
+  <si>
+    <t>WillPower2</t>
+  </si>
+  <si>
+    <t>HealPower2</t>
+  </si>
+  <si>
+    <t>FireTargetMaxRange</t>
+  </si>
+  <si>
+    <t>FireCostConSaveDC</t>
+  </si>
+  <si>
+    <t>1d20</t>
+  </si>
+  <si>
+    <t>FireCostConSaveDCHalfFailRange</t>
+  </si>
+  <si>
+    <t>FireSpreadPerRound</t>
+  </si>
+  <si>
+    <t>FireIgniteDC</t>
+  </si>
+  <si>
+    <t>VisionRange</t>
+  </si>
+  <si>
+    <t>fire points</t>
+  </si>
+  <si>
+    <t>1d20 (Adv)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -527,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -537,21 +646,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,7 +991,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -890,11 +1001,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1096,11 +1207,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1198,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -1242,7 +1353,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1298,11 +1409,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1480,26 +1591,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134592FA-46C7-4490-B8BE-DC20D051C225}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.06640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>34</v>
+        <v>134</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" t="s">
@@ -1510,20 +1621,20 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -1538,21 +1649,21 @@
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
         <v>6</v>
@@ -1564,10 +1675,10 @@
     </row>
     <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
         <v>22</v>
@@ -1577,33 +1688,37 @@
         <v>0.40833333333333333</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="C6" s="2">
+        <v>39</v>
+      </c>
       <c r="D6">
         <f>5*C6/100</f>
-        <v>0</v>
+        <v>1.95</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
         <v>9</v>
@@ -1614,7 +1729,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2">
         <v>3</v>
@@ -1624,25 +1739,25 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" s="2">
         <v>100</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="9">
         <f>H7-H8</f>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
@@ -1655,14 +1770,14 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="2">
-        <v>50</v>
-      </c>
-      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
         <f>(1+(J7/100))</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1670,7 +1785,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>
@@ -1680,24 +1795,24 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11">
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9">
         <f>(IF(H6=0,D12,1))+IF(H5="y",D13,0)</f>
-        <v>2</v>
-      </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <f>(D4-1)*D8</f>
@@ -1706,22 +1821,22 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12">
+      <c r="G10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10">
         <f>(D4-((J8*D15)*H6/D8))*J9</f>
-        <v>12</v>
-      </c>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <f>D4*D8</f>
@@ -1730,32 +1845,32 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="13">
+      <c r="G11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="11">
         <f>IF(J10&gt;0,ROUNDDOWN((D4/J10)*D9,0),"OoB")</f>
-        <v>6</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="11">
+        <v>39</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="9">
         <f>IF(J10&gt;0,J11*6/60,"OoB")</f>
-        <v>0.6</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>45</v>
+        <v>3.9</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -1765,105 +1880,923 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J12">
         <f>IF(J10&gt;0,ROUNDDOWN(MAX(1,J11*(J8*D14)),0),"OoB")</f>
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="K12" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12">
+        <v>36</v>
+      </c>
+      <c r="L12" s="19">
         <f>IF(J10&gt;0,J12*6/60,"OoB")</f>
-        <v>1.8</v>
+        <v>15.6</v>
       </c>
       <c r="M12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" s="8">
         <f>IF(J10&gt;0,1/J12,0)</f>
-        <v>5.5555555555555552E-2</v>
+        <v>6.41025641025641E-3</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
       <c r="D14">
         <f>MIN(20,21-C14)/10</f>
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14">
+        <v>61</v>
+      </c>
+      <c r="J14" s="3">
         <f>IF(J10&gt;0,J12*D5,"OoB")</f>
-        <v>7.35</v>
+        <v>63.699999999999996</v>
+      </c>
+      <c r="K14" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C15" s="2">
+        <v>15</v>
+      </c>
       <c r="D15">
         <f>MIN(20,21-C15)/10</f>
-        <v>2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C17" s="14"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>136</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28">
+        <v>-7</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="20"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="3"/>
+      <c r="G30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="17">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="3"/>
+      <c r="G31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="20"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="3"/>
+      <c r="G32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="17">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D33" s="20">
+        <v>70</v>
+      </c>
+      <c r="E33" s="18">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="G33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D34" s="20">
+        <v>0</v>
+      </c>
+      <c r="E34" s="18">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="G34" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="G2:K2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="G2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD424A96-8909-42CC-88FF-139D8D2AB429}">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5">
+        <f>C5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="E6" t="str">
+        <f>IF(C6=1,"Seconds",IF(C6=2,"Minutes",IF(C6=3,"Hours",IF(C6=4,"Days",IF(C6=5,"Weeks",IF(C6=6,"Months",IF(C6=7,"Years",IF(C6=8,"Decades",IF(C6=9,"Centuries",IF(C6=10,"Millenia","INVALID"))))))))))</f>
+        <v>INVALID</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <f>E6</f>
+        <v>INVALID</v>
+      </c>
+      <c r="G7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8">
+        <f>D7*C8/100</f>
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f>E6</f>
+        <v>INVALID</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9">
+        <f>D7*C9/100</f>
+        <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <f>E6</f>
+        <v>INVALID</v>
+      </c>
+      <c r="G9" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="7">
+        <f>MIN(0,MAX(-D7,-(H7*D8)+(H8*D9)))</f>
+        <v>0</v>
+      </c>
+      <c r="K9" t="str">
+        <f>E6</f>
+        <v>INVALID</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>C6</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <f>J9*7</f>
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f>C11+D10</f>
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="7">
+        <f>J10/30</f>
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f>ROUNDUP(C12+D10/2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="2">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <f>ROUNDUP(C13+D10/2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <f>ROUNDUP((D4*C14*D10/75)/5,0)*5</f>
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14">
+        <f>H12+H13</f>
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f>C15</f>
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f>C16</f>
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="2">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="2">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <f>C17</f>
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17">
+        <f>ROUNDUP(ROUNDDOWN(H16/(D11/2),0)*(D11/2)/D11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="14">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <f>11-C18</f>
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>C20</f>
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="2">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <f>C21</f>
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <f>ROUNDUP(C22/2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="25" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f>C25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="2">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <f>C26*D25</f>
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <f>MAX(1,20-C27-D25)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28">
+        <f>20-C28+ROUNDUP(D25/2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29">
+        <f>C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <f>C30+D25</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="2">
+        <v>9</v>
+      </c>
+      <c r="D32">
+        <f>C31+(MOD(C32,D25))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="2">
+        <v>82</v>
+      </c>
+      <c r="D34">
+        <f>C33+ROUNDUP(D25*C34/100,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="2">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <f>C35*D25</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36">
+        <f>MAX(1,POWER(D25,2)/10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37">
+        <f>10+D25</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38">
+        <f>120+(18*10)</f>
+        <v>300</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7192FBE2-AD5D-4485-BBB2-1057D825DAB4}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection sqref="A1:K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1877,30 +2810,30 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1915,14 +2848,14 @@
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
@@ -1937,12 +2870,12 @@
     </row>
     <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="15">
+        <v>77</v>
+      </c>
+      <c r="C5" s="12">
         <v>3</v>
       </c>
       <c r="D5">
@@ -1952,10 +2885,10 @@
     </row>
     <row r="6" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -1964,17 +2897,15 @@
         <f>IF(C6=1,"Seconds",IF(C6=2,"Minutes",IF(C6=3,"Hours",IF(C6=4,"Days",IF(C6=5,"Weeks",IF(C6=6,"Months",IF(C6=7,"Years",IF(C6=8,"Decades",IF(C6=9,"Centuries",IF(C6=10,"Millenia","INVALID"))))))))))</f>
         <v>Weeks</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="16">
+        <v>69</v>
+      </c>
+      <c r="C7" s="13">
         <v>8</v>
       </c>
       <c r="D7">
@@ -1986,19 +2917,19 @@
         <v>Weeks</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2">
         <v>19</v>
@@ -2012,21 +2943,21 @@
         <v>Weeks</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="17">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2">
         <v>40</v>
       </c>
       <c r="D9">
@@ -2038,7 +2969,7 @@
         <v>Weeks</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J9" s="7">
         <f>MIN(0,MAX(-D7,-(H7*D8)+(H8*D9)))</f>
@@ -2051,10 +2982,10 @@
     </row>
     <row r="10" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2">
         <v>7</v>
@@ -2063,22 +2994,20 @@
         <f>C6</f>
         <v>5</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
       <c r="J10" s="7">
         <f>J9*7</f>
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -2088,24 +3017,22 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+        <v>36</v>
+      </c>
       <c r="J11" s="7">
         <f>J10/30</f>
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -2115,26 +3042,26 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H12" s="2">
         <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="19">
+        <v>46</v>
+      </c>
+      <c r="C13" s="14">
         <v>2</v>
       </c>
       <c r="D13">
@@ -2142,26 +3069,26 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H13" s="2">
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="17">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2">
         <v>5</v>
       </c>
       <c r="D14">
@@ -2172,22 +3099,22 @@
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J14">
         <f>H12+H13</f>
         <v>17</v>
       </c>
       <c r="K14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2">
         <v>4</v>
@@ -2197,17 +3124,15 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
         <v>95</v>
-      </c>
-      <c r="B16" t="s">
-        <v>96</v>
       </c>
       <c r="C16" s="2">
         <v>8</v>
@@ -2217,24 +3142,24 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H16" s="2">
         <v>4</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>37</v>
+      <c r="I16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="2">
         <v>8</v>
@@ -2244,29 +3169,27 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
-      </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
+        <v>117</v>
+      </c>
       <c r="J17">
         <f>ROUNDUP(ROUNDDOWN(H16/(D11/2),0)*(D11/2)/D11,0)</f>
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="19">
+        <v>77</v>
+      </c>
+      <c r="C18" s="14">
         <v>7</v>
       </c>
       <c r="D18">
@@ -2274,15 +3197,15 @@
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2">
         <v>3</v>
@@ -2292,15 +3215,15 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2">
         <v>3</v>
@@ -2310,17 +3233,17 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="17">
+        <v>99</v>
+      </c>
+      <c r="C21" s="2">
         <v>6</v>
       </c>
       <c r="D21">
@@ -2328,17 +3251,17 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="17">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2">
         <v>3</v>
       </c>
       <c r="D22">
@@ -2346,24 +3269,24 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2376,7 +3299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604DF105-CA70-4A4B-93B9-9180A75A341E}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>